<commit_message>
edit music player view (kompozytory)
</commit_message>
<xml_diff>
--- a/autorToSong.xlsx
+++ b/autorToSong.xlsx
@@ -74,7 +74,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -90,9 +90,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -130,7 +130,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -202,7 +202,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -352,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,7 +393,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G106" si="0">$D$1&amp;A2&amp;$E$1&amp;B2&amp;$F$1</f>
+        <f t="shared" ref="G2:G107" si="0">$D$1&amp;A2&amp;$E$1&amp;B2&amp;$F$1</f>
         <v>INSERT INTO `e-spiewnik`.`SongToComposer` (`Id`, `Songs_Id`, `Composers_Id`) VALUES (NULL, '2','1');</v>
       </c>
     </row>
@@ -1643,6 +1643,18 @@
       <c r="G106" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO `e-spiewnik`.`SongToComposer` (`Id`, `Songs_Id`, `Composers_Id`) VALUES (NULL, '103','3');</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>104</v>
+      </c>
+      <c r="B107">
+        <v>3</v>
+      </c>
+      <c r="G107" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `e-spiewnik`.`SongToComposer` (`Id`, `Songs_Id`, `Composers_Id`) VALUES (NULL, '104','3');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>